<commit_message>
0.3.0 - Added as_date, various bug fixes and added tests
</commit_message>
<xml_diff>
--- a/spec/data/import_test_data.xlsx
+++ b/spec/data/import_test_data.xlsx
@@ -77,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -408,6 +409,17 @@
         <v>2.4</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B5" s="1">
+        <v>42036</v>
+      </c>
+      <c r="C5" s="1">
+        <v>42036</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>